<commit_message>
python integration test and readme is done!!!!
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bernh\Nextcloud\Projekte\1901-TechnikumWien\LVs\BIF3-SWEN1_WS2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel_work\Documents\FH\FH\swen_01\FH_swen01_MonsterTradingCardGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654F465-E96B-4F58-9905-119C7AA41DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EFF794-1FB0-4592-ADE4-5C76B24E8EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-15" windowWidth="25440" windowHeight="15390" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -309,7 +309,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -597,7 +597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -607,43 +607,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="5" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
@@ -651,76 +651,76 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="4" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>14</v>
       </c>
@@ -731,12 +731,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>17</v>
       </c>
@@ -744,7 +744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>18</v>
       </c>
@@ -752,7 +752,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
@@ -760,7 +760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>20</v>
       </c>
@@ -768,7 +768,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>21</v>
       </c>
@@ -776,7 +776,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
@@ -784,14 +784,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B28"/>
       <c r="C28"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>24</v>
       </c>
@@ -799,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>25</v>
       </c>
@@ -807,7 +807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>26</v>
       </c>
@@ -815,7 +815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -823,7 +823,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>28</v>
       </c>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -839,7 +839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>30</v>
       </c>
@@ -848,14 +848,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B38"/>
       <c r="C38"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>32</v>
       </c>
@@ -863,7 +863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>33</v>
       </c>
@@ -871,7 +871,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>34</v>
       </c>
@@ -879,7 +879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>35</v>
       </c>
@@ -887,29 +887,32 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B44"/>
       <c r="C44" s="6"/>
     </row>
-    <row r="46" spans="1:3" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>46</v>
       </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
       <c r="C47" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>38</v>
       </c>
@@ -917,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>39</v>
       </c>
@@ -925,7 +928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>40</v>
       </c>
@@ -933,7 +936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>41</v>
       </c>
@@ -941,21 +944,24 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="B52">
+        <v>0.5</v>
+      </c>
       <c r="C52" s="6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A54" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B54" s="2">
         <f>IF(MIN(B9:B16)=1,SUM(B21:B52),0)</f>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="C54" s="2">
         <f>SUM(C21:C52)</f>
@@ -974,6 +980,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100495F7CC252815B47896F98900E10984C" ma:contentTypeVersion="2" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="afe1b3b164495dc81fdbcdcad6ec8b68">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="207955a2-a3fc-4582-b2ea-e4c7d1fb6048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3b6a42bf87c3f8727d31c248fc1697f6" ns2:_="">
     <xsd:import namespace="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
@@ -1105,22 +1126,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0824ED0-660A-437B-A039-7835C5DD208D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1136,28 +1166,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B871BF9-5772-4B74-B6DF-7878EF29873D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FFD0135-03B1-4A6A-9DC8-B4D791C0671E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="207955a2-a3fc-4582-b2ea-e4c7d1fb6048"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>